<commit_message>
update SDR, update statistics
</commit_message>
<xml_diff>
--- a/data/2020-Artedi-SDR-Oxygen.xlsx
+++ b/data/2020-Artedi-SDR-Oxygen.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Taylor/CloudStation/Cisco-Climate-Change/NA-Coregonine-Latitude/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Taylor/CloudStation/Cisco-Climate-Change/Coregonine-Latitude-Embryo/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D06EF30-0069-8942-AB72-6EC467FD386D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E986FA11-440F-F144-B01B-2BEA6C035169}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="10000" windowHeight="16600" xr2:uid="{507B9C5B-6304-6341-95EF-95E900B4AD86}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="32">
   <si>
     <t>population</t>
   </si>
@@ -126,6 +126,9 @@
   </si>
   <si>
     <t>hatch.date</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -487,7 +490,7 @@
   <dimension ref="A1:E193"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D180" sqref="D180"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -526,6 +529,9 @@
       <c r="D2">
         <v>1</v>
       </c>
+      <c r="E2" s="1">
+        <v>43865</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -582,6 +588,9 @@
       <c r="D6">
         <v>1</v>
       </c>
+      <c r="E6" s="1">
+        <v>43865</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -596,6 +605,9 @@
       <c r="D7">
         <v>1</v>
       </c>
+      <c r="E7" s="1">
+        <v>43865</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -624,6 +636,9 @@
       <c r="D9">
         <v>1</v>
       </c>
+      <c r="E9" s="1">
+        <v>43865</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
@@ -652,6 +667,9 @@
       <c r="D11">
         <v>1</v>
       </c>
+      <c r="E11" s="1">
+        <v>43865</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
@@ -680,6 +698,9 @@
       <c r="D13">
         <v>1</v>
       </c>
+      <c r="E13" s="1">
+        <v>43848</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
@@ -694,6 +715,9 @@
       <c r="D14">
         <v>1</v>
       </c>
+      <c r="E14" s="1">
+        <v>43865</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
@@ -708,6 +732,9 @@
       <c r="D15">
         <v>1</v>
       </c>
+      <c r="E15" s="1">
+        <v>43865</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
@@ -722,6 +749,9 @@
       <c r="D16">
         <v>1</v>
       </c>
+      <c r="E16" s="1">
+        <v>43848</v>
+      </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
@@ -750,6 +780,9 @@
       <c r="D18">
         <v>1</v>
       </c>
+      <c r="E18" s="1">
+        <v>43865</v>
+      </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
@@ -778,6 +811,9 @@
       <c r="D20">
         <v>1</v>
       </c>
+      <c r="E20" s="1">
+        <v>43865</v>
+      </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
@@ -791,6 +827,9 @@
       </c>
       <c r="D21">
         <v>0</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>